<commit_message>
update output imaging assay
</commit_message>
<xml_diff>
--- a/templates/dataplant/3ASY05_Imaging.xlsx
+++ b/templates/dataplant/3ASY05_Imaging.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin\source\repos\SWATE_templates\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martin\Documents\GitHub\Swate-templates_FORK\templates\dataplant\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74580EBA-EE2F-4C3B-9501-6560B76EC82A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{731ADB0C-07E3-41CF-BE1D-DBFBA82D0306}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="19110" windowHeight="12450" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6165" yWindow="2340" windowWidth="22785" windowHeight="14535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="3ASY05_Imaging" sheetId="1" r:id="rId1"/>
@@ -127,7 +127,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="163">
   <si>
     <t>Source Name</t>
   </si>
@@ -613,13 +613,16 @@
   </si>
   <si>
     <t>Authors Role Term Source REF</t>
+  </si>
+  <si>
+    <t>Raw Data File</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -634,12 +637,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -800,7 +797,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -810,6 +806,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -881,7 +878,7 @@
     <tableColumn id="42" xr3:uid="{B5E0717A-AE44-415C-86DE-6E24BA5A9600}" name="Parameter [Image file path]"/>
     <tableColumn id="43" xr3:uid="{38FC1F12-3A80-4B6A-A380-7D91DE7DA03F}" name="Term Source REF (NFDI4PSO:1000120)"/>
     <tableColumn id="44" xr3:uid="{F63FF2CB-0409-4F44-9E83-8AFA1D23BBCA}" name="Term Accession Number (NFDI4PSO:1000120)"/>
-    <tableColumn id="45" xr3:uid="{6446AF9A-A0B5-4A14-A8EE-47CFCB268B72}" name="Data File Name"/>
+    <tableColumn id="2" xr3:uid="{09643D96-CC5D-4919-8933-E1A5E83C2C54}" name="Raw Data File"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1185,7 +1182,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="665" row="2">
+  <wetp:taskpane dockstate="right" visibility="0" width="350" row="3">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
   <wetp:taskpane dockstate="right" visibility="0" width="638" row="2">
@@ -1218,54 +1215,56 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AR4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
+      <selection activeCell="AO2" sqref="AO2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37" customWidth="1"/>
+    <col min="2" max="2" width="32.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="36.7109375" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="68" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="30.85546875" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="37.85546875" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="67.5703125" customWidth="1"/>
+    <col min="8" max="8" width="31.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="30.85546875" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="37.85546875" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="56.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="36.7109375" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="56.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="31.42578125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="36.7109375" hidden="1" customWidth="1"/>
     <col min="16" max="16" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="30.140625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="36.7109375" hidden="1" customWidth="1"/>
     <col min="19" max="19" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="36.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="36.42578125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="36.7109375" hidden="1" customWidth="1"/>
     <col min="22" max="22" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="38" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="38.28515625" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="36.7109375" hidden="1" customWidth="1"/>
     <col min="25" max="25" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="26" max="26" width="37.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="38" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="36.7109375" hidden="1" customWidth="1"/>
     <col min="28" max="28" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="29" max="29" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="25.5703125" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="36.7109375" hidden="1" customWidth="1"/>
     <col min="31" max="31" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="32" max="32" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="27.28515625" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="36.7109375" hidden="1" customWidth="1"/>
     <col min="34" max="34" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="35" max="35" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="45.140625" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="36.7109375" hidden="1" customWidth="1"/>
     <col min="37" max="37" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="38" max="38" width="44.85546875" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="33" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="36.7109375" hidden="1" customWidth="1"/>
     <col min="40" max="40" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="41" max="41" width="28" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="28.28515625" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="36.7109375" hidden="1" customWidth="1"/>
     <col min="43" max="43" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="44" max="44" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:44" x14ac:dyDescent="0.25">
@@ -1399,7 +1398,7 @@
         <v>42</v>
       </c>
       <c r="AR1" t="s">
-        <v>43</v>
+        <v>162</v>
       </c>
     </row>
     <row r="2" spans="1:44" x14ac:dyDescent="0.25">
@@ -1484,6 +1483,7 @@
       <c r="AQ2" t="s">
         <v>154</v>
       </c>
+      <c r="AR2" s="13"/>
     </row>
     <row r="3" spans="1:44" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
@@ -1531,6 +1531,7 @@
       <c r="AQ3" t="s">
         <v>154</v>
       </c>
+      <c r="AR3" s="13"/>
     </row>
     <row r="4" spans="1:44" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
@@ -1542,6 +1543,7 @@
       <c r="D4" t="s">
         <v>154</v>
       </c>
+      <c r="AR4" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1555,16 +1557,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D26667D-8A82-460C-AF9D-703E927267EC}">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="57.140625" style="10" customWidth="1"/>
-    <col min="3" max="3" width="12" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="11.42578125" style="10"/>
+    <col min="1" max="1" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="57.140625" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1771,8 +1772,8 @@
       <c r="A27" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="B27" s="13"/>
-      <c r="C27" s="13"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -1805,470 +1806,470 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="J1" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="K1" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="L1" s="10" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12" t="s">
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12" t="s">
+      <c r="H3" s="11"/>
+      <c r="I3" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="J3" s="12" t="s">
+      <c r="J3" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="K3" s="12" t="s">
+      <c r="K3" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="L3" s="12"/>
+      <c r="L3" s="11"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12" t="s">
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12" t="s">
+      <c r="H4" s="11"/>
+      <c r="I4" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="J4" s="12" t="s">
+      <c r="J4" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="K4" s="12" t="s">
+      <c r="K4" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="L4" s="12"/>
+      <c r="L4" s="11"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12" t="s">
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12" t="s">
+      <c r="H5" s="11"/>
+      <c r="I5" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="J5" s="12" t="s">
+      <c r="J5" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="K5" s="12" t="s">
+      <c r="K5" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="L5" s="12"/>
+      <c r="L5" s="11"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12" t="s">
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12" t="s">
+      <c r="H6" s="11"/>
+      <c r="I6" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="J6" s="12" t="s">
+      <c r="J6" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="K6" s="12" t="s">
+      <c r="K6" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="L6" s="12"/>
+      <c r="L6" s="11"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12" t="s">
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12" t="s">
+      <c r="H7" s="11"/>
+      <c r="I7" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="J7" s="12" t="s">
+      <c r="J7" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="K7" s="12" t="s">
+      <c r="K7" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="L7" s="12"/>
+      <c r="L7" s="11"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12" t="s">
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12" t="s">
+      <c r="H8" s="11"/>
+      <c r="I8" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="J8" s="12" t="s">
+      <c r="J8" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="K8" s="12" t="s">
+      <c r="K8" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="L8" s="12"/>
+      <c r="L8" s="11"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12" t="s">
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12" t="s">
+      <c r="H9" s="11"/>
+      <c r="I9" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="J9" s="12" t="s">
+      <c r="J9" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="K9" s="12" t="s">
+      <c r="K9" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="L9" s="12"/>
+      <c r="L9" s="11"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12" t="s">
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12" t="s">
+      <c r="H10" s="11"/>
+      <c r="I10" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="J10" s="12" t="s">
+      <c r="J10" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="K10" s="12" t="s">
+      <c r="K10" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="L10" s="12"/>
+      <c r="L10" s="11"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12" t="s">
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12" t="s">
+      <c r="H11" s="11"/>
+      <c r="I11" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="J11" s="12" t="s">
+      <c r="J11" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="K11" s="12" t="s">
+      <c r="K11" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="L11" s="12"/>
+      <c r="L11" s="11"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D12" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12" t="s">
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="J12" s="12"/>
-      <c r="K12" s="12"/>
-      <c r="L12" s="12"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D13" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12" t="s">
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="J13" s="12"/>
-      <c r="K13" s="12"/>
-      <c r="L13" s="12"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="D14" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12" t="s">
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12" t="s">
+      <c r="H14" s="11"/>
+      <c r="I14" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="J14" s="12" t="s">
+      <c r="J14" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="K14" s="12" t="s">
+      <c r="K14" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="L14" s="12"/>
+      <c r="L14" s="11"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D15" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12" t="s">
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="J15" s="12"/>
-      <c r="K15" s="12"/>
-      <c r="L15" s="12"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="11"/>
+      <c r="L15" s="11"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D16" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12" t="s">
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="J16" s="12"/>
-      <c r="K16" s="12"/>
-      <c r="L16" s="12"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="11"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="10" t="s">
         <v>156</v>
       </c>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="12"/>
-      <c r="K17" s="12"/>
-      <c r="L17" s="12"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -2300,498 +2301,498 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="J1" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="K1" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="L1" s="10" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12" t="s">
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12" t="s">
+      <c r="H3" s="11"/>
+      <c r="I3" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="J3" s="12" t="s">
+      <c r="J3" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="K3" s="12" t="s">
+      <c r="K3" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="L3" s="12"/>
+      <c r="L3" s="11"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12" t="s">
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12" t="s">
+      <c r="H4" s="11"/>
+      <c r="I4" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="J4" s="12" t="s">
+      <c r="J4" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="K4" s="12" t="s">
+      <c r="K4" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="L4" s="12"/>
+      <c r="L4" s="11"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12" t="s">
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12" t="s">
+      <c r="H5" s="11"/>
+      <c r="I5" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="J5" s="12" t="s">
+      <c r="J5" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="K5" s="12" t="s">
+      <c r="K5" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="L5" s="12"/>
+      <c r="L5" s="11"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12" t="s">
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12" t="s">
+      <c r="H6" s="11"/>
+      <c r="I6" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="J6" s="12" t="s">
+      <c r="J6" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="K6" s="12" t="s">
+      <c r="K6" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="L6" s="12"/>
+      <c r="L6" s="11"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12" t="s">
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12" t="s">
+      <c r="H7" s="11"/>
+      <c r="I7" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="J7" s="12" t="s">
+      <c r="J7" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="K7" s="12" t="s">
+      <c r="K7" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="L7" s="12"/>
+      <c r="L7" s="11"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12" t="s">
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="H8" s="12" t="s">
+      <c r="H8" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="I8" s="12" t="s">
+      <c r="I8" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="J8" s="12" t="s">
+      <c r="J8" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="K8" s="12"/>
-      <c r="L8" s="12"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12" t="s">
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12" t="s">
+      <c r="H9" s="11"/>
+      <c r="I9" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="J9" s="12" t="s">
+      <c r="J9" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="K9" s="12" t="s">
+      <c r="K9" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="L9" s="12"/>
+      <c r="L9" s="11"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12" t="s">
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12" t="s">
+      <c r="H10" s="11"/>
+      <c r="I10" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="J10" s="12" t="s">
+      <c r="J10" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="K10" s="12" t="s">
+      <c r="K10" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="L10" s="12"/>
+      <c r="L10" s="11"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12" t="s">
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12" t="s">
+      <c r="H11" s="11"/>
+      <c r="I11" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="J11" s="12" t="s">
+      <c r="J11" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="K11" s="12" t="s">
+      <c r="K11" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="L11" s="12"/>
+      <c r="L11" s="11"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D12" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12" t="s">
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="H12" s="12" t="s">
+      <c r="H12" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="I12" s="12" t="s">
+      <c r="I12" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="J12" s="12" t="s">
+      <c r="J12" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="K12" s="12" t="s">
+      <c r="K12" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="L12" s="12"/>
+      <c r="L12" s="11"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D13" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12" t="s">
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="H13" s="12" t="s">
+      <c r="H13" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="I13" s="12" t="s">
+      <c r="I13" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="J13" s="12" t="s">
+      <c r="J13" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="K13" s="12" t="s">
+      <c r="K13" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="L13" s="12"/>
+      <c r="L13" s="11"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="D14" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12" t="s">
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12" t="s">
+      <c r="H14" s="11"/>
+      <c r="I14" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="J14" s="12" t="s">
+      <c r="J14" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="K14" s="12" t="s">
+      <c r="K14" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="L14" s="12"/>
+      <c r="L14" s="11"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D15" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12" t="s">
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11" t="s">
         <v>135</v>
       </c>
-      <c r="H15" s="12" t="s">
+      <c r="H15" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="I15" s="12" t="s">
+      <c r="I15" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="J15" s="12" t="s">
+      <c r="J15" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="K15" s="12"/>
-      <c r="L15" s="12"/>
+      <c r="K15" s="11"/>
+      <c r="L15" s="11"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D16" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12" t="s">
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="H16" s="12" t="s">
+      <c r="H16" s="11" t="s">
         <v>138</v>
       </c>
-      <c r="I16" s="12" t="s">
+      <c r="I16" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="J16" s="12" t="s">
+      <c r="J16" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="K16" s="12"/>
-      <c r="L16" s="12"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="11"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="12"/>
-      <c r="K17" s="12"/>
-      <c r="L17" s="12"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
replace nfdi4pso terms in imaging assay template
</commit_message>
<xml_diff>
--- a/templates/dataplant/3ASY05_Imaging.xlsx
+++ b/templates/dataplant/3ASY05_Imaging.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martin\Documents\GitHub\Swate-templates_FORK\templates\dataplant\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stella Eggels\sciebo - Eggels, Stella (s.eggels@fz-juelich.de)@fz-juelich.sciebo.de\SE\DataPLANT\ARCs und SWATE\ersatz von nfdi4pso\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{731ADB0C-07E3-41CF-BE1D-DBFBA82D0306}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE1D9CFE-D78F-4447-A461-2CADCBCB30E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6165" yWindow="2340" windowWidth="22785" windowHeight="14535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="3ASY05_Imaging" sheetId="1" r:id="rId1"/>
@@ -50,75 +50,75 @@
   <commentList>
     <comment ref="A1" authorId="0" shapeId="0" xr:uid="{764CF3E1-B993-49DB-9C5C-1661BE8D9836}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
     The unique identifier of this template. It will be auto generated.
-Reply:
+Antwort:
     id=e60ba840-a310-4ea9-8a1e-5f4c979473f3</t>
       </text>
     </comment>
     <comment ref="A2" authorId="1" shapeId="0" xr:uid="{E6E71A1A-EC05-4048-AC80-F5D20E0E32CC}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
     The name of the Swate template.</t>
       </text>
     </comment>
     <comment ref="A3" authorId="2" shapeId="0" xr:uid="{A9AE190C-EEFA-42D3-9D64-C393CAEE790C}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
     The current version of this template in SemVer notation.</t>
       </text>
     </comment>
     <comment ref="A4" authorId="3" shapeId="0" xr:uid="{F8C2A495-F446-4980-90C0-232C4B92674B}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
     The description of this template. Use few sentences for succinctness.</t>
       </text>
     </comment>
     <comment ref="A5" authorId="4" shapeId="0" xr:uid="{80E34628-7986-4C05-8491-94EDE97209D3}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
     The name of the template associated organisation. "DataPLANT" will trigger the "DataPLANT" batch of honor for the template.</t>
       </text>
     </comment>
     <comment ref="A6" authorId="5" shapeId="0" xr:uid="{8E5959C0-E30B-4A8A-96C9-EE48C532C18F}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
     The name of the Swate annotation table in the workbook of the template's excel file.</t>
       </text>
     </comment>
     <comment ref="A7" authorId="6" shapeId="0" xr:uid="{3D3C88B7-7282-4217-AD57-AA111CF70AB9}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
     A list of all ERs (endpoint repositories) targeted with this template. ERs are realized as Terms: &lt;term ref here&gt;</t>
       </text>
     </comment>
     <comment ref="A11" authorId="7" shapeId="0" xr:uid="{41F9B4C8-C1D9-4A75-9F7E-FBFD0250A152}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
     A list of all tags associated with this template. Tags are realized as Terms: &lt;term ref here&gt;</t>
       </text>
     </comment>
     <comment ref="A15" authorId="8" shapeId="0" xr:uid="{0269C758-6BF2-4C3A-A396-7FFD8C1334D2}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
     The author(s) of this template.</t>
       </text>
     </comment>
@@ -127,7 +127,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="173">
   <si>
     <t>Source Name</t>
   </si>
@@ -135,12 +135,6 @@
     <t>Parameter [target compartment]</t>
   </si>
   <si>
-    <t>Term Source REF (NFDI4PSO:1000121)</t>
-  </si>
-  <si>
-    <t>Term Accession Number (NFDI4PSO:1000121)</t>
-  </si>
-  <si>
     <t>Parameter [microscope]</t>
   </si>
   <si>
@@ -162,102 +156,36 @@
     <t>Parameter [Objective]</t>
   </si>
   <si>
-    <t>Term Source REF (NFDI4PSO:1000142)</t>
-  </si>
-  <si>
-    <t>Term Accession Number (NFDI4PSO:1000142)</t>
-  </si>
-  <si>
     <t>Parameter [Magnification]</t>
   </si>
   <si>
-    <t>Term Source REF (NFDI4PSO:1000140)</t>
-  </si>
-  <si>
-    <t>Term Accession Number (NFDI4PSO:1000140)</t>
-  </si>
-  <si>
     <t>Parameter [Microscope filter]</t>
   </si>
   <si>
-    <t>Term Source REF (NFDI4PSO:1000125)</t>
-  </si>
-  <si>
-    <t>Term Accession Number (NFDI4PSO:1000125)</t>
-  </si>
-  <si>
     <t>Parameter [Imaging Software Name]</t>
   </si>
   <si>
-    <t>Term Source REF (NFDI4PSO:1000122)</t>
-  </si>
-  <si>
-    <t>Term Accession Number (NFDI4PSO:1000122)</t>
-  </si>
-  <si>
     <t>Parameter [Imaging Software Settings]</t>
   </si>
   <si>
-    <t>Term Source REF (NFDI4PSO:1000124)</t>
-  </si>
-  <si>
-    <t>Term Accession Number (NFDI4PSO:1000124)</t>
-  </si>
-  <si>
     <t>Parameter [Imaging Software Version]</t>
   </si>
   <si>
-    <t>Term Source REF (NFDI4PSO:1000123)</t>
-  </si>
-  <si>
-    <t>Term Accession Number (NFDI4PSO:1000123)</t>
-  </si>
-  <si>
     <t>Parameter [Assay Name]</t>
   </si>
   <si>
-    <t>Term Source REF (NFDI4PSO:1000127)</t>
-  </si>
-  <si>
-    <t>Term Accession Number (NFDI4PSO:1000127)</t>
-  </si>
-  <si>
     <t>Parameter [Dataset Name]</t>
   </si>
   <si>
-    <t>Term Source REF (NFDI4PSO:1000126)</t>
-  </si>
-  <si>
-    <t>Term Accession Number (NFDI4PSO:1000126)</t>
-  </si>
-  <si>
     <t>Parameter [Image Dimensionality]</t>
   </si>
   <si>
-    <t>Term Source REF (NFDI4PSO:1000141)</t>
-  </si>
-  <si>
-    <t>Term Accession Number (NFDI4PSO:1000141)</t>
-  </si>
-  <si>
     <t>Parameter [Raw data file format]</t>
   </si>
   <si>
-    <t>Term Source REF (NFDI4PSO:0000021)</t>
-  </si>
-  <si>
-    <t>Term Accession Number (NFDI4PSO:0000021)</t>
-  </si>
-  <si>
     <t>Parameter [Image file path]</t>
   </si>
   <si>
-    <t>Term Source REF (NFDI4PSO:1000120)</t>
-  </si>
-  <si>
-    <t>Term Accession Number (NFDI4PSO:1000120)</t>
-  </si>
-  <si>
     <t>Data File Name</t>
   </si>
   <si>
@@ -396,9 +324,6 @@
     <t>Review comments</t>
   </si>
   <si>
-    <t>NFDI4PSO</t>
-  </si>
-  <si>
     <t>n</t>
   </si>
   <si>
@@ -420,12 +345,6 @@
     <t>cv | s</t>
   </si>
   <si>
-    <t>NFDI4PSO:1000121</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NFDI4PSO_1000121</t>
-  </si>
-  <si>
     <t>OBI:0400169</t>
   </si>
   <si>
@@ -438,72 +357,6 @@
     <t>http://purl.obolibrary.org/obo/OBI_0001048</t>
   </si>
   <si>
-    <t>NFDI4PSO:1000142</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NFDI4PSO_1000142</t>
-  </si>
-  <si>
-    <t>NFDI4PSO:1000140</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NFDI4PSO_1000140</t>
-  </si>
-  <si>
-    <t>NFDI4PSO:1000125</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NFDI4PSO_1000125</t>
-  </si>
-  <si>
-    <t>NFDI4PSO:1000122</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NFDI4PSO_1000122</t>
-  </si>
-  <si>
-    <t>NFDI4PSO:1000124</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NFDI4PSO_1000124</t>
-  </si>
-  <si>
-    <t>NFDI4PSO:1000123</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NFDI4PSO_1000123</t>
-  </si>
-  <si>
-    <t>NFDI4PSO:1000127</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NFDI4PSO_1000127</t>
-  </si>
-  <si>
-    <t>NFDI4PSO:1000126</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NFDI4PSO_1000126</t>
-  </si>
-  <si>
-    <t>NFDI4PSO:1000141</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NFDI4PSO_1000141</t>
-  </si>
-  <si>
-    <t>NFDI4PSO:0000021</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NFDI4PSO_0000021</t>
-  </si>
-  <si>
-    <t>NFDI4PSO:1000120</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NFDI4PSO_1000120</t>
-  </si>
-  <si>
     <t>Protocol_image acquisition_and_feature_extraction_Description</t>
   </si>
   <si>
@@ -594,9 +447,6 @@
     <t>user-specific</t>
   </si>
   <si>
-    <t>1.0.2</t>
-  </si>
-  <si>
     <t>Data File+A13:A17 Name</t>
   </si>
   <si>
@@ -616,13 +466,193 @@
   </si>
   <si>
     <t>Raw Data File</t>
+  </si>
+  <si>
+    <t>Term Source REF (DPBO:1000121)</t>
+  </si>
+  <si>
+    <t>Term Accession Number (DPBO:1000121)</t>
+  </si>
+  <si>
+    <t>Term Source REF (OME:Objective)</t>
+  </si>
+  <si>
+    <t>Term Accession Number (OME:Objective)</t>
+  </si>
+  <si>
+    <t>Parameter [magnification]</t>
+  </si>
+  <si>
+    <t>Term Source REF (DPBO:1000140)</t>
+  </si>
+  <si>
+    <t>Term Accession Number (DPBO:1000140)</t>
+  </si>
+  <si>
+    <t>Parameter [microscope filter]</t>
+  </si>
+  <si>
+    <t>Term Source REF (DPBO:1000125)</t>
+  </si>
+  <si>
+    <t>Term Accession Number (DPBO:1000125)</t>
+  </si>
+  <si>
+    <t>Term Source REF (NCIT:C175898)</t>
+  </si>
+  <si>
+    <t>Term Accession Number (NCIT:C175898)</t>
+  </si>
+  <si>
+    <t>Parameter [imaging software settings]</t>
+  </si>
+  <si>
+    <t>Term Source REF (DPBO:1000124)</t>
+  </si>
+  <si>
+    <t>Term Accession Number (DPBO:1000124)</t>
+  </si>
+  <si>
+    <t>Parameter [imaging software version]</t>
+  </si>
+  <si>
+    <t>Term Source REF (DPBO:1000123)</t>
+  </si>
+  <si>
+    <t>Term Accession Number (DPBO:1000123)</t>
+  </si>
+  <si>
+    <t>Term Source REF (NCIT:C178857)</t>
+  </si>
+  <si>
+    <t>Term Accession Number (NCIT:C178857)</t>
+  </si>
+  <si>
+    <t>Parameter [dataset name]</t>
+  </si>
+  <si>
+    <t>Term Source REF (DPBO:1000126)</t>
+  </si>
+  <si>
+    <t>Term Accession Number (DPBO:1000126)</t>
+  </si>
+  <si>
+    <t>Parameter [image dimensionality]</t>
+  </si>
+  <si>
+    <t>Term Source REF (DPBO:1000141)</t>
+  </si>
+  <si>
+    <t>Term Accession Number (DPBO:1000141)</t>
+  </si>
+  <si>
+    <t>Parameter [raw data file format]</t>
+  </si>
+  <si>
+    <t>Term Source REF (DPBO:0000021)</t>
+  </si>
+  <si>
+    <t>Term Accession Number (DPBO:0000021)</t>
+  </si>
+  <si>
+    <t>Parameter [image file path]</t>
+  </si>
+  <si>
+    <t>Term Source REF (DPBO:1000120)</t>
+  </si>
+  <si>
+    <t>Term Accession Number (DPBO:1000120)</t>
+  </si>
+  <si>
+    <t>1.0.3</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C178857</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C175898</t>
+  </si>
+  <si>
+    <t>OME</t>
+  </si>
+  <si>
+    <t>DPBO</t>
+  </si>
+  <si>
+    <t>NCIT</t>
+  </si>
+  <si>
+    <t>DPBO:1000121</t>
+  </si>
+  <si>
+    <t>OME:Objective</t>
+  </si>
+  <si>
+    <t>DPBO:1000140</t>
+  </si>
+  <si>
+    <t>DPBO:1000125</t>
+  </si>
+  <si>
+    <t>NCIT:C175898</t>
+  </si>
+  <si>
+    <t>DPBO:1000124</t>
+  </si>
+  <si>
+    <t>DPBO:1000123</t>
+  </si>
+  <si>
+    <t>NCIT:C178857</t>
+  </si>
+  <si>
+    <t>DPBO:1000126</t>
+  </si>
+  <si>
+    <t>DPBO:1000141</t>
+  </si>
+  <si>
+    <t>DPBO:0000021</t>
+  </si>
+  <si>
+    <t>DPBO:1000120</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/DPBO_1000121</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OME_Objective</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/DPBO_1000140</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/DPBO_1000125</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/DPBO_1000124</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/DPBO_1000123</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/DPBO_1000126</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/DPBO_1000141</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/DPBO_0000021</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/DPBO_1000120</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -634,6 +664,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFF5F5F5"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -765,10 +803,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -807,11 +846,118 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="34">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -836,48 +982,48 @@
   <autoFilter ref="A1:AR4" xr:uid="{4DCB7EF1-A6AB-404C-8A31-1D96F4226C41}"/>
   <tableColumns count="44">
     <tableColumn id="1" xr3:uid="{9752695C-1854-41AD-AAD5-2B5A9E07A795}" name="Source Name"/>
-    <tableColumn id="3" xr3:uid="{466E59A6-1A78-4FF3-B96E-553DFBBF24B0}" name="Parameter [target compartment]"/>
-    <tableColumn id="4" xr3:uid="{721C3BFE-F7F6-41D4-BC30-77AF5EDACD9C}" name="Term Source REF (NFDI4PSO:1000121)"/>
-    <tableColumn id="5" xr3:uid="{8E8ED479-1221-49F4-BA8A-A9B0B9524D70}" name="Term Accession Number (NFDI4PSO:1000121)"/>
+    <tableColumn id="3" xr3:uid="{40CC8C83-0EEB-4801-8726-14FB8C2B7920}" name="Parameter [target compartment]"/>
+    <tableColumn id="4" xr3:uid="{5E565679-31FA-47E7-B5BF-2CE4B5FA47E6}" name="Term Source REF (DPBO:1000121)" dataDxfId="33"/>
+    <tableColumn id="5" xr3:uid="{8D055D4D-F5A1-4E5A-80E0-01630691592C}" name="Term Accession Number (DPBO:1000121)" dataDxfId="32"/>
     <tableColumn id="6" xr3:uid="{EB48CCAD-BB1F-45B3-BE28-BFFC53CDFF52}" name="Parameter [microscope]"/>
     <tableColumn id="7" xr3:uid="{86D2366F-44A6-44EB-86DB-1BAFA55057B7}" name="Term Source REF (OBI:0400169)"/>
     <tableColumn id="8" xr3:uid="{FE94E9F1-BC5D-4F3C-A022-00283B0774E0}" name="Term Accession Number (OBI:0400169)"/>
     <tableColumn id="9" xr3:uid="{978D0B3F-8DAE-4263-8413-471030EC24A0}" name="Parameter [digital camera]"/>
     <tableColumn id="10" xr3:uid="{60C87E9F-DE23-4036-93EF-1283BCDA1DB7}" name="Term Source REF (OBI:0001048)"/>
     <tableColumn id="11" xr3:uid="{6DFB85BA-6491-4D88-832A-DDA123822AC3}" name="Term Accession Number (OBI:0001048)"/>
-    <tableColumn id="12" xr3:uid="{DE655DEB-2DBD-4056-9B70-32C19B1B32BC}" name="Parameter [Objective]"/>
-    <tableColumn id="13" xr3:uid="{CFF5EA87-F8D5-4F3A-87ED-B6A910AF4C93}" name="Term Source REF (NFDI4PSO:1000142)"/>
-    <tableColumn id="14" xr3:uid="{1B89059D-C583-4305-858C-2FB6BE1CA1FA}" name="Term Accession Number (NFDI4PSO:1000142)"/>
-    <tableColumn id="15" xr3:uid="{C3166C1C-663F-4870-8BA9-3E3B34332A86}" name="Parameter [Magnification]"/>
-    <tableColumn id="16" xr3:uid="{C76363AB-E8CB-437A-AEF6-2ED79A3C2D0D}" name="Term Source REF (NFDI4PSO:1000140)"/>
-    <tableColumn id="17" xr3:uid="{4744A927-BD2A-4474-A2C7-1D0E3A0094E3}" name="Term Accession Number (NFDI4PSO:1000140)"/>
-    <tableColumn id="18" xr3:uid="{C23730C6-5319-4193-96BD-62250F99885A}" name="Parameter [Microscope filter]"/>
-    <tableColumn id="19" xr3:uid="{E91F3609-3E22-47E3-BFB2-FFE2A706CC33}" name="Term Source REF (NFDI4PSO:1000125)"/>
-    <tableColumn id="20" xr3:uid="{8C8227A9-DDD8-4EB1-AFB5-F902436EC423}" name="Term Accession Number (NFDI4PSO:1000125)"/>
-    <tableColumn id="21" xr3:uid="{C00CE8EB-49C7-49B5-806B-94650FE9E295}" name="Parameter [Imaging Software Name]"/>
-    <tableColumn id="22" xr3:uid="{3FA1CC2D-D3EC-48CF-BD6F-3CA1E04654CF}" name="Term Source REF (NFDI4PSO:1000122)"/>
-    <tableColumn id="23" xr3:uid="{5DAE9692-9B05-43D5-B11C-17BE03D3DAB9}" name="Term Accession Number (NFDI4PSO:1000122)"/>
-    <tableColumn id="24" xr3:uid="{D0B8E006-9C25-4DFC-8254-77542AA09D4A}" name="Parameter [Imaging Software Settings]"/>
-    <tableColumn id="25" xr3:uid="{AE4AD6BA-FEB6-42A3-9D0A-30985C06BC46}" name="Term Source REF (NFDI4PSO:1000124)"/>
-    <tableColumn id="26" xr3:uid="{8EF33BC8-20B0-44DA-BAB7-1E6DFD72CDDB}" name="Term Accession Number (NFDI4PSO:1000124)"/>
-    <tableColumn id="27" xr3:uid="{B7B5963B-5845-47EE-8EC6-B060B4A4FAA9}" name="Parameter [Imaging Software Version]"/>
-    <tableColumn id="28" xr3:uid="{D8870D76-6B80-4F40-B23C-E0F2FCB2DE0C}" name="Term Source REF (NFDI4PSO:1000123)"/>
-    <tableColumn id="29" xr3:uid="{130C2C6C-BC2F-484F-A495-96DED53764D9}" name="Term Accession Number (NFDI4PSO:1000123)"/>
-    <tableColumn id="30" xr3:uid="{1490FB8A-CE7C-4CE5-AFCB-21BCAB722515}" name="Parameter [Assay Name]"/>
-    <tableColumn id="31" xr3:uid="{C5AE1E06-A9CD-4D15-A2A7-A5640F28FCE7}" name="Term Source REF (NFDI4PSO:1000127)"/>
-    <tableColumn id="32" xr3:uid="{2350C537-DA2A-4028-86FE-1BB3DBFB986A}" name="Term Accession Number (NFDI4PSO:1000127)"/>
-    <tableColumn id="33" xr3:uid="{ADCFC852-6C59-47E4-8F14-BA07046520BB}" name="Parameter [Dataset Name]"/>
-    <tableColumn id="34" xr3:uid="{0136F41A-86B4-4CEC-9528-633F5A48CB28}" name="Term Source REF (NFDI4PSO:1000126)"/>
-    <tableColumn id="35" xr3:uid="{707298C0-B1E5-467F-8ABA-210A6C77EDB3}" name="Term Accession Number (NFDI4PSO:1000126)"/>
-    <tableColumn id="36" xr3:uid="{65BE7308-C23B-42EE-94AE-EF8684CEC843}" name="Parameter [Image Dimensionality]"/>
-    <tableColumn id="37" xr3:uid="{5D65F238-CBF5-4ECD-9635-550ADEC683CE}" name="Term Source REF (NFDI4PSO:1000141)"/>
-    <tableColumn id="38" xr3:uid="{455A21F8-8182-4D1F-BC4B-10F7CC764D87}" name="Term Accession Number (NFDI4PSO:1000141)"/>
-    <tableColumn id="39" xr3:uid="{4D0C5618-53F3-43EB-8A0C-A461CAD2A81B}" name="Parameter [Raw data file format]"/>
-    <tableColumn id="40" xr3:uid="{0F9FCE10-60DC-4493-9E57-802E6EC44FE8}" name="Term Source REF (NFDI4PSO:0000021)"/>
-    <tableColumn id="41" xr3:uid="{FCE8F397-D636-4522-B80D-371CF84A0144}" name="Term Accession Number (NFDI4PSO:0000021)"/>
-    <tableColumn id="42" xr3:uid="{B5E0717A-AE44-415C-86DE-6E24BA5A9600}" name="Parameter [Image file path]"/>
-    <tableColumn id="43" xr3:uid="{38FC1F12-3A80-4B6A-A380-7D91DE7DA03F}" name="Term Source REF (NFDI4PSO:1000120)"/>
-    <tableColumn id="44" xr3:uid="{F63FF2CB-0409-4F44-9E83-8AFA1D23BBCA}" name="Term Accession Number (NFDI4PSO:1000120)"/>
+    <tableColumn id="12" xr3:uid="{7A40B5CF-F991-456A-ADB9-26F154C9FBDC}" name="Parameter [Objective]"/>
+    <tableColumn id="13" xr3:uid="{AC052AAC-B89F-4C73-9BED-522BC55DBDA6}" name="Term Source REF (OME:Objective)" dataDxfId="31"/>
+    <tableColumn id="14" xr3:uid="{1CA94A6A-10B2-48BD-A777-CE6DB727EC23}" name="Term Accession Number (OME:Objective)" dataDxfId="30"/>
+    <tableColumn id="15" xr3:uid="{1561C3A3-F09D-4DAB-BBB3-8436AE9A5676}" name="Parameter [magnification]" dataDxfId="29"/>
+    <tableColumn id="16" xr3:uid="{1EDF7FFB-342A-4503-96B1-5D84DB12D564}" name="Term Source REF (DPBO:1000140)" dataDxfId="28"/>
+    <tableColumn id="17" xr3:uid="{2993C4E5-A782-431F-9098-578B1BBC3488}" name="Term Accession Number (DPBO:1000140)" dataDxfId="27"/>
+    <tableColumn id="18" xr3:uid="{97A8BFD8-54CE-405D-ABDA-7B03390AE19B}" name="Parameter [microscope filter]" dataDxfId="26"/>
+    <tableColumn id="19" xr3:uid="{C6F61E8F-2DC6-4758-9424-B8B7D81E7EA6}" name="Term Source REF (DPBO:1000125)" dataDxfId="25"/>
+    <tableColumn id="20" xr3:uid="{2A291869-CD32-40BD-A503-D0F51897FBE4}" name="Term Accession Number (DPBO:1000125)" dataDxfId="24"/>
+    <tableColumn id="21" xr3:uid="{47330B61-2AC8-4D01-A266-C4FD13912E4D}" name="Parameter [Imaging Software Name]" dataDxfId="23"/>
+    <tableColumn id="22" xr3:uid="{30B94354-076A-4086-B426-2A05B74F3324}" name="Term Source REF (NCIT:C175898)" dataDxfId="22"/>
+    <tableColumn id="23" xr3:uid="{6E0E52A2-E01C-479D-885C-B096B2FEB454}" name="Term Accession Number (NCIT:C175898)" dataDxfId="21"/>
+    <tableColumn id="24" xr3:uid="{4AD012C0-5E1B-40AD-BDCB-F58F3E6EFF0B}" name="Parameter [imaging software settings]" dataDxfId="20"/>
+    <tableColumn id="25" xr3:uid="{5968384C-432F-40CD-8292-F4F967F5EB59}" name="Term Source REF (DPBO:1000124)" dataDxfId="19"/>
+    <tableColumn id="26" xr3:uid="{5A57BAE1-64A5-41EF-8D03-E05EBF0AD915}" name="Term Accession Number (DPBO:1000124)" dataDxfId="18"/>
+    <tableColumn id="27" xr3:uid="{9A6110EA-F8F7-4970-A13B-2BC0C3186A79}" name="Parameter [imaging software version]" dataDxfId="17"/>
+    <tableColumn id="28" xr3:uid="{6A33607D-8215-488B-B7EA-583FE414954A}" name="Term Source REF (DPBO:1000123)" dataDxfId="16"/>
+    <tableColumn id="29" xr3:uid="{0C65F9A0-96FA-402C-9CFD-C155591DB2C9}" name="Term Accession Number (DPBO:1000123)" dataDxfId="15"/>
+    <tableColumn id="30" xr3:uid="{3AB90BF6-ADDE-4E5B-B0E9-512AC7422454}" name="Parameter [Assay Name]" dataDxfId="14"/>
+    <tableColumn id="31" xr3:uid="{4E4B0CAD-89C4-4DED-ABCB-4FC3413D7444}" name="Term Source REF (NCIT:C178857)" dataDxfId="13"/>
+    <tableColumn id="32" xr3:uid="{5EB1743D-80CA-46F3-A330-15C33DF56FBE}" name="Term Accession Number (NCIT:C178857)" dataDxfId="12"/>
+    <tableColumn id="33" xr3:uid="{13BEFD3D-B29A-44D6-AA48-FC3E1837E89E}" name="Parameter [dataset name]" dataDxfId="11"/>
+    <tableColumn id="34" xr3:uid="{E8FBABC7-396E-4CE9-8974-C0700687F8BA}" name="Term Source REF (DPBO:1000126)" dataDxfId="10"/>
+    <tableColumn id="35" xr3:uid="{B4F0E0AB-4856-4704-8DE2-8AD782C3163F}" name="Term Accession Number (DPBO:1000126)" dataDxfId="9"/>
+    <tableColumn id="36" xr3:uid="{2808B2D8-44FE-49CC-9D3E-638CEE69D65F}" name="Parameter [image dimensionality]" dataDxfId="8"/>
+    <tableColumn id="37" xr3:uid="{9BCD6DBD-91CE-4853-A011-D1460D8DD636}" name="Term Source REF (DPBO:1000141)" dataDxfId="7"/>
+    <tableColumn id="38" xr3:uid="{524183DF-B7C7-4608-915B-03505C24FB2D}" name="Term Accession Number (DPBO:1000141)" dataDxfId="6"/>
+    <tableColumn id="39" xr3:uid="{43B43B5D-DD5A-4CDC-9026-99A9A159984C}" name="Parameter [raw data file format]" dataDxfId="5"/>
+    <tableColumn id="40" xr3:uid="{5A887AC0-5CB2-4850-9DAF-C070797FA5F8}" name="Term Source REF (DPBO:0000021)" dataDxfId="4"/>
+    <tableColumn id="41" xr3:uid="{C7980730-F2F6-49EC-874F-04AA9A2CDC80}" name="Term Accession Number (DPBO:0000021)" dataDxfId="3"/>
+    <tableColumn id="42" xr3:uid="{805395D8-A83F-4BA2-B5B2-FEB99EED6552}" name="Parameter [image file path]" dataDxfId="2"/>
+    <tableColumn id="43" xr3:uid="{E07371D7-FD8E-4F0D-84BB-0F6B1EB8D44E}" name="Term Source REF (DPBO:1000120)" dataDxfId="1"/>
+    <tableColumn id="44" xr3:uid="{9F691610-47B6-4D79-B2EC-8FF7C00D8302}" name="Term Accession Number (DPBO:1000120)" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{09643D96-CC5D-4919-8933-E1A5E83C2C54}" name="Raw Data File"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1182,7 +1328,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="350" row="3">
+  <wetp:taskpane dockstate="right" visibility="0" width="451" row="0">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
   <wetp:taskpane dockstate="right" visibility="0" width="638" row="2">
@@ -1215,59 +1361,59 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AR4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
-      <selection activeCell="AO2" sqref="AO2"/>
+    <sheetView tabSelected="1" topLeftCell="AI1" workbookViewId="0">
+      <selection activeCell="AO25" sqref="AO25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.7109375" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="68" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.85546875" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="37.85546875" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.85546875" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="37.85546875" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="56.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="36.7109375" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="31.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="36.7109375" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="36.7109375" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="36.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="36.7109375" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="38.28515625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="36.7109375" hidden="1" customWidth="1"/>
-    <col min="25" max="25" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="26" max="26" width="38" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="36.7109375" hidden="1" customWidth="1"/>
-    <col min="28" max="28" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="29" max="29" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="36.7109375" hidden="1" customWidth="1"/>
-    <col min="31" max="31" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="32" max="32" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="36.7109375" hidden="1" customWidth="1"/>
-    <col min="34" max="34" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="35" max="35" width="45.140625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="36.7109375" hidden="1" customWidth="1"/>
-    <col min="37" max="37" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="38" max="38" width="33" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="36.7109375" hidden="1" customWidth="1"/>
-    <col min="40" max="40" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="41" max="41" width="28.28515625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="36.7109375" hidden="1" customWidth="1"/>
-    <col min="43" max="43" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="44" max="44" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.6640625" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="38.109375" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="61.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.88671875" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="37.88671875" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="29.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.88671875" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="37.88671875" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="32" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="38.44140625" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="25.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="31.6640625" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="38.109375" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="28" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="31.6640625" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="38.109375" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="34.44140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="31" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="37.44140625" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="35.5546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="31.6640625" hidden="1" customWidth="1"/>
+    <col min="25" max="25" width="38.109375" hidden="1" customWidth="1"/>
+    <col min="26" max="26" width="35.21875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="31.6640625" hidden="1" customWidth="1"/>
+    <col min="28" max="28" width="38.109375" hidden="1" customWidth="1"/>
+    <col min="29" max="29" width="24.21875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="31" hidden="1" customWidth="1"/>
+    <col min="31" max="31" width="37.44140625" hidden="1" customWidth="1"/>
+    <col min="32" max="32" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="31.6640625" hidden="1" customWidth="1"/>
+    <col min="34" max="34" width="38.109375" hidden="1" customWidth="1"/>
+    <col min="35" max="35" width="32" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="31.6640625" hidden="1" customWidth="1"/>
+    <col min="37" max="37" width="38.109375" hidden="1" customWidth="1"/>
+    <col min="38" max="38" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="31.6640625" hidden="1" customWidth="1"/>
+    <col min="40" max="40" width="38.109375" hidden="1" customWidth="1"/>
+    <col min="41" max="41" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="31.6640625" hidden="1" customWidth="1"/>
+    <col min="43" max="43" width="38.109375" hidden="1" customWidth="1"/>
+    <col min="44" max="44" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1275,273 +1421,494 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
       <c r="L1" t="s">
+        <v>115</v>
+      </c>
+      <c r="M1" t="s">
+        <v>116</v>
+      </c>
+      <c r="N1" t="s">
+        <v>117</v>
+      </c>
+      <c r="O1" t="s">
+        <v>118</v>
+      </c>
+      <c r="P1" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>120</v>
+      </c>
+      <c r="R1" t="s">
+        <v>121</v>
+      </c>
+      <c r="S1" t="s">
+        <v>122</v>
+      </c>
+      <c r="T1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" t="s">
+      <c r="U1" t="s">
+        <v>123</v>
+      </c>
+      <c r="V1" t="s">
+        <v>124</v>
+      </c>
+      <c r="W1" t="s">
+        <v>125</v>
+      </c>
+      <c r="X1" t="s">
+        <v>126</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>127</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>129</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>130</v>
+      </c>
+      <c r="AC1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" t="s">
-        <v>21</v>
-      </c>
-      <c r="W1" t="s">
-        <v>22</v>
-      </c>
-      <c r="X1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>28</v>
-      </c>
       <c r="AD1" t="s">
-        <v>29</v>
+        <v>131</v>
       </c>
       <c r="AE1" t="s">
-        <v>30</v>
+        <v>132</v>
       </c>
       <c r="AF1" t="s">
-        <v>31</v>
+        <v>133</v>
       </c>
       <c r="AG1" t="s">
-        <v>32</v>
+        <v>134</v>
       </c>
       <c r="AH1" t="s">
-        <v>33</v>
+        <v>135</v>
       </c>
       <c r="AI1" t="s">
-        <v>34</v>
+        <v>136</v>
       </c>
       <c r="AJ1" t="s">
-        <v>35</v>
+        <v>137</v>
       </c>
       <c r="AK1" t="s">
-        <v>36</v>
+        <v>138</v>
       </c>
       <c r="AL1" t="s">
-        <v>37</v>
+        <v>139</v>
       </c>
       <c r="AM1" t="s">
-        <v>38</v>
+        <v>140</v>
       </c>
       <c r="AN1" t="s">
-        <v>39</v>
+        <v>141</v>
       </c>
       <c r="AO1" t="s">
-        <v>40</v>
+        <v>142</v>
       </c>
       <c r="AP1" t="s">
-        <v>41</v>
+        <v>143</v>
       </c>
       <c r="AQ1" t="s">
-        <v>42</v>
+        <v>144</v>
       </c>
       <c r="AR1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="2" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>139</v>
-      </c>
-      <c r="C2" t="s">
-        <v>154</v>
-      </c>
-      <c r="D2" t="s">
-        <v>154</v>
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:44" x14ac:dyDescent="0.3">
+      <c r="B2" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>53</v>
       </c>
       <c r="E2" t="s">
-        <v>140</v>
+        <v>91</v>
       </c>
       <c r="F2" t="s">
-        <v>154</v>
+        <v>105</v>
       </c>
       <c r="G2" t="s">
-        <v>154</v>
+        <v>105</v>
       </c>
       <c r="H2" t="s">
-        <v>141</v>
+        <v>92</v>
       </c>
       <c r="I2" t="s">
-        <v>154</v>
+        <v>105</v>
       </c>
       <c r="J2" t="s">
-        <v>154</v>
-      </c>
-      <c r="K2" t="s">
-        <v>142</v>
-      </c>
-      <c r="L2" t="s">
-        <v>154</v>
-      </c>
-      <c r="M2" t="s">
-        <v>154</v>
-      </c>
-      <c r="N2" t="s">
-        <v>143</v>
-      </c>
-      <c r="O2" t="s">
-        <v>154</v>
-      </c>
-      <c r="P2" t="s">
-        <v>154</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>144</v>
-      </c>
-      <c r="R2" t="s">
-        <v>154</v>
-      </c>
-      <c r="S2" t="s">
-        <v>154</v>
-      </c>
-      <c r="T2" t="s">
-        <v>145</v>
-      </c>
-      <c r="U2" t="s">
-        <v>154</v>
-      </c>
-      <c r="V2" t="s">
-        <v>154</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>146</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>154</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>154</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>147</v>
-      </c>
-      <c r="AP2" t="s">
-        <v>154</v>
-      </c>
-      <c r="AQ2" t="s">
-        <v>154</v>
+        <v>105</v>
+      </c>
+      <c r="K2" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="L2" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="M2" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="N2" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="O2" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="P2" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q2" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="R2" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="S2" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="T2" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="U2" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="V2" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="W2" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="X2" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y2" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="Z2" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="AA2" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB2" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="AC2" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD2" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="AE2" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="AF2" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="AG2" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="AH2" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="AI2" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="AJ2" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="AK2" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="AL2" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="AM2" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="AN2" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="AO2" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="AP2" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="AQ2" s="13" t="s">
+        <v>53</v>
       </c>
       <c r="AR2" s="13"/>
     </row>
-    <row r="3" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>148</v>
-      </c>
-      <c r="C3" t="s">
-        <v>154</v>
-      </c>
-      <c r="D3" t="s">
-        <v>154</v>
+    <row r="3" spans="1:44" x14ac:dyDescent="0.3">
+      <c r="B3" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>53</v>
       </c>
       <c r="E3" t="s">
-        <v>149</v>
+        <v>100</v>
       </c>
       <c r="F3" t="s">
-        <v>154</v>
+        <v>105</v>
       </c>
       <c r="G3" t="s">
-        <v>154</v>
+        <v>105</v>
       </c>
       <c r="H3" t="s">
-        <v>150</v>
+        <v>101</v>
       </c>
       <c r="I3" t="s">
-        <v>154</v>
+        <v>105</v>
       </c>
       <c r="J3" t="s">
-        <v>154</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>151</v>
-      </c>
-      <c r="R3" t="s">
-        <v>154</v>
-      </c>
-      <c r="S3" t="s">
-        <v>154</v>
-      </c>
-      <c r="AL3" t="s">
-        <v>152</v>
-      </c>
-      <c r="AP3" t="s">
-        <v>154</v>
-      </c>
-      <c r="AQ3" t="s">
-        <v>154</v>
+        <v>105</v>
+      </c>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="M3" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="N3" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="O3" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="P3" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q3" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="R3" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="S3" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="T3" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="U3" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="V3" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="W3" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="X3" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y3" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="Z3" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="AA3" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB3" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="AC3" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD3" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="AE3" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="AF3" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="AG3" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="AH3" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="AI3" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="AJ3" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="AK3" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="AL3" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="AM3" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="AN3" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="AO3" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="AP3" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="AQ3" s="13" t="s">
+        <v>53</v>
       </c>
       <c r="AR3" s="13"/>
     </row>
-    <row r="4" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>153</v>
-      </c>
-      <c r="C4" t="s">
-        <v>154</v>
-      </c>
-      <c r="D4" t="s">
-        <v>154</v>
+    <row r="4" spans="1:44" x14ac:dyDescent="0.3">
+      <c r="B4" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="M4" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="N4" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="O4" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="P4" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q4" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="R4" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="S4" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="T4" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="U4" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="V4" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="W4" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="X4" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y4" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="Z4" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="AA4" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB4" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="AC4" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD4" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="AE4" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="AF4" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="AG4" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="AH4" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="AI4" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="AJ4" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="AK4" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="AL4" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="AM4" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="AN4" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="AO4" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="AP4" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="AQ4" s="13" t="s">
+        <v>53</v>
       </c>
       <c r="AR4" s="13"/>
     </row>
@@ -1558,219 +1925,219 @@
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="57.140625" customWidth="1"/>
+    <col min="1" max="1" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="57.109375" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="8" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>71</v>
+        <v>47</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>52</v>
+        <v>28</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>53</v>
+        <v>29</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>54</v>
+        <v>30</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>55</v>
+        <v>31</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>56</v>
+        <v>32</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>57</v>
+        <v>33</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>59</v>
+        <v>35</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>73</v>
+        <v>49</v>
       </c>
       <c r="C16" s="6"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>60</v>
+        <v>36</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>74</v>
+        <v>50</v>
       </c>
       <c r="C17" s="2"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>66</v>
+        <v>42</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>158</v>
+        <v>108</v>
       </c>
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>159</v>
+        <v>109</v>
       </c>
       <c r="B25" s="9"/>
       <c r="C25" s="9"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>160</v>
+        <v>110</v>
       </c>
       <c r="B26" s="9"/>
       <c r="C26" s="9"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
-        <v>161</v>
+        <v>111</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="12"/>
@@ -1785,65 +2152,65 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{784E0D4F-11C2-4FD1-95D0-67870F1968D1}">
   <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:A18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="50.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="46.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="50.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.88671875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="99" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" customWidth="1"/>
-    <col min="9" max="9" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5546875" customWidth="1"/>
+    <col min="9" max="9" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>78</v>
+        <v>54</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>79</v>
+        <v>55</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>80</v>
+        <v>56</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>81</v>
+        <v>57</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>82</v>
+        <v>58</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>83</v>
+        <v>59</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>84</v>
+        <v>60</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>85</v>
+        <v>61</v>
       </c>
       <c r="J1" s="10" t="s">
-        <v>86</v>
+        <v>62</v>
       </c>
       <c r="K1" s="10" t="s">
-        <v>87</v>
+        <v>63</v>
       </c>
       <c r="L1" s="10" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
@@ -1859,405 +2226,405 @@
       <c r="K2" s="11"/>
       <c r="L2" s="11"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>97</v>
+        <v>151</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>98</v>
+        <v>149</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>163</v>
       </c>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
       <c r="G3" s="11" t="s">
-        <v>125</v>
+        <v>76</v>
       </c>
       <c r="H3" s="11"/>
       <c r="I3" s="11" t="s">
-        <v>91</v>
+        <v>66</v>
       </c>
       <c r="J3" s="11" t="s">
-        <v>92</v>
+        <v>67</v>
       </c>
       <c r="K3" s="11" t="s">
-        <v>93</v>
+        <v>68</v>
       </c>
       <c r="L3" s="11"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>99</v>
+        <v>72</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>100</v>
+        <v>69</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>73</v>
       </c>
       <c r="E4" s="11"/>
       <c r="F4" s="11"/>
       <c r="G4" s="11" t="s">
-        <v>125</v>
+        <v>76</v>
       </c>
       <c r="H4" s="11"/>
       <c r="I4" s="11" t="s">
-        <v>91</v>
+        <v>66</v>
       </c>
       <c r="J4" s="11" t="s">
-        <v>92</v>
+        <v>67</v>
       </c>
       <c r="K4" s="11" t="s">
-        <v>93</v>
+        <v>68</v>
       </c>
       <c r="L4" s="11"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>101</v>
+        <v>74</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>94</v>
+        <v>69</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>102</v>
+        <v>75</v>
       </c>
       <c r="E5" s="11"/>
       <c r="F5" s="11"/>
       <c r="G5" s="11" t="s">
-        <v>125</v>
+        <v>76</v>
       </c>
       <c r="H5" s="11"/>
       <c r="I5" s="11" t="s">
-        <v>91</v>
+        <v>66</v>
       </c>
       <c r="J5" s="11" t="s">
-        <v>92</v>
+        <v>67</v>
       </c>
       <c r="K5" s="11" t="s">
-        <v>93</v>
+        <v>68</v>
       </c>
       <c r="L5" s="11"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>103</v>
+        <v>152</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>104</v>
+        <v>148</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>164</v>
       </c>
       <c r="E6" s="11"/>
       <c r="F6" s="11"/>
       <c r="G6" s="11" t="s">
-        <v>125</v>
+        <v>76</v>
       </c>
       <c r="H6" s="11"/>
       <c r="I6" s="11" t="s">
-        <v>91</v>
+        <v>66</v>
       </c>
       <c r="J6" s="11" t="s">
-        <v>92</v>
+        <v>67</v>
       </c>
       <c r="K6" s="11" t="s">
-        <v>93</v>
+        <v>68</v>
       </c>
       <c r="L6" s="11"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>105</v>
+        <v>153</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>106</v>
+        <v>149</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>165</v>
       </c>
       <c r="E7" s="11"/>
       <c r="F7" s="11"/>
       <c r="G7" s="11" t="s">
-        <v>125</v>
+        <v>76</v>
       </c>
       <c r="H7" s="11"/>
       <c r="I7" s="11" t="s">
-        <v>91</v>
+        <v>66</v>
       </c>
       <c r="J7" s="11" t="s">
-        <v>92</v>
+        <v>67</v>
       </c>
       <c r="K7" s="11" t="s">
-        <v>93</v>
+        <v>68</v>
       </c>
       <c r="L7" s="11"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>107</v>
+        <v>154</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>108</v>
+        <v>149</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>166</v>
       </c>
       <c r="E8" s="11"/>
       <c r="F8" s="11"/>
       <c r="G8" s="11" t="s">
-        <v>125</v>
+        <v>76</v>
       </c>
       <c r="H8" s="11"/>
       <c r="I8" s="11" t="s">
-        <v>91</v>
+        <v>66</v>
       </c>
       <c r="J8" s="11" t="s">
-        <v>92</v>
+        <v>67</v>
       </c>
       <c r="K8" s="11" t="s">
-        <v>93</v>
+        <v>68</v>
       </c>
       <c r="L8" s="11"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>109</v>
+        <v>155</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>110</v>
+        <v>150</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>147</v>
       </c>
       <c r="E9" s="11"/>
       <c r="F9" s="11"/>
       <c r="G9" s="11" t="s">
-        <v>125</v>
+        <v>76</v>
       </c>
       <c r="H9" s="11"/>
       <c r="I9" s="11" t="s">
-        <v>91</v>
+        <v>66</v>
       </c>
       <c r="J9" s="11" t="s">
-        <v>92</v>
+        <v>67</v>
       </c>
       <c r="K9" s="11" t="s">
-        <v>93</v>
+        <v>68</v>
       </c>
       <c r="L9" s="11"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>111</v>
+        <v>156</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>112</v>
+        <v>149</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>167</v>
       </c>
       <c r="E10" s="11"/>
       <c r="F10" s="11"/>
       <c r="G10" s="11" t="s">
-        <v>125</v>
+        <v>76</v>
       </c>
       <c r="H10" s="11"/>
       <c r="I10" s="11" t="s">
-        <v>91</v>
+        <v>66</v>
       </c>
       <c r="J10" s="11" t="s">
-        <v>92</v>
+        <v>67</v>
       </c>
       <c r="K10" s="11" t="s">
-        <v>93</v>
+        <v>68</v>
       </c>
       <c r="L10" s="11"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>113</v>
+        <v>157</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>114</v>
+        <v>149</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>168</v>
       </c>
       <c r="E11" s="11"/>
       <c r="F11" s="11"/>
       <c r="G11" s="11" t="s">
-        <v>125</v>
+        <v>76</v>
       </c>
       <c r="H11" s="11"/>
       <c r="I11" s="11" t="s">
-        <v>91</v>
+        <v>66</v>
       </c>
       <c r="J11" s="11" t="s">
-        <v>92</v>
+        <v>67</v>
       </c>
       <c r="K11" s="11" t="s">
-        <v>93</v>
+        <v>68</v>
       </c>
       <c r="L11" s="11"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>115</v>
+        <v>158</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>116</v>
+        <v>150</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>146</v>
       </c>
       <c r="E12" s="11"/>
       <c r="F12" s="11"/>
       <c r="G12" s="11"/>
       <c r="H12" s="11"/>
       <c r="I12" s="11" t="s">
-        <v>90</v>
+        <v>65</v>
       </c>
       <c r="J12" s="11"/>
       <c r="K12" s="11"/>
       <c r="L12" s="11"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>117</v>
+        <v>159</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>118</v>
+        <v>149</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>169</v>
       </c>
       <c r="E13" s="11"/>
       <c r="F13" s="11"/>
       <c r="G13" s="11"/>
       <c r="H13" s="11"/>
       <c r="I13" s="11" t="s">
-        <v>90</v>
+        <v>65</v>
       </c>
       <c r="J13" s="11"/>
       <c r="K13" s="11"/>
       <c r="L13" s="11"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>119</v>
+        <v>160</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>120</v>
+        <v>149</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>170</v>
       </c>
       <c r="E14" s="11"/>
       <c r="F14" s="11"/>
       <c r="G14" s="11" t="s">
-        <v>125</v>
+        <v>76</v>
       </c>
       <c r="H14" s="11"/>
       <c r="I14" s="11" t="s">
-        <v>91</v>
+        <v>66</v>
       </c>
       <c r="J14" s="11" t="s">
-        <v>92</v>
+        <v>67</v>
       </c>
       <c r="K14" s="11" t="s">
-        <v>93</v>
+        <v>68</v>
       </c>
       <c r="L14" s="11"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>121</v>
+        <v>161</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>122</v>
+        <v>149</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>171</v>
       </c>
       <c r="E15" s="11"/>
       <c r="F15" s="11"/>
       <c r="G15" s="11"/>
       <c r="H15" s="11"/>
       <c r="I15" s="11" t="s">
-        <v>90</v>
+        <v>65</v>
       </c>
       <c r="J15" s="11"/>
       <c r="K15" s="11"/>
       <c r="L15" s="11"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>123</v>
+        <v>162</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>124</v>
+        <v>149</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>172</v>
       </c>
       <c r="E16" s="11"/>
       <c r="F16" s="11"/>
       <c r="G16" s="11"/>
       <c r="H16" s="11"/>
       <c r="I16" s="11" t="s">
-        <v>90</v>
+        <v>65</v>
       </c>
       <c r="J16" s="11"/>
       <c r="K16" s="11"/>
       <c r="L16" s="11"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
-        <v>156</v>
+        <v>106</v>
       </c>
       <c r="B17" s="11"/>
       <c r="C17" s="11"/>
@@ -2272,6 +2639,21 @@
       <c r="L17" s="11"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D9" r:id="rId1" xr:uid="{6B66B74F-7786-4EC6-9D59-AFE728A7D9F0}"/>
+    <hyperlink ref="D12" r:id="rId2" xr:uid="{AFB7745F-8311-4A3F-B8A7-CE02AC9D7A5A}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{2D6C8A2A-FDE8-421A-82AC-F5936B2D6B61}"/>
+    <hyperlink ref="D3" r:id="rId4" xr:uid="{52353B34-5324-41AA-8FA6-2460907F88C4}"/>
+    <hyperlink ref="D6" r:id="rId5" xr:uid="{BD166AE5-641E-4200-93C9-D66325E39ADE}"/>
+    <hyperlink ref="D7" r:id="rId6" xr:uid="{DED58E12-2AD0-47D7-9029-2D6241F334C3}"/>
+    <hyperlink ref="D8" r:id="rId7" xr:uid="{64CC7B5A-9521-4267-B20E-A7D28EC0321A}"/>
+    <hyperlink ref="D10" r:id="rId8" xr:uid="{B219C1F1-632F-474B-9262-57C17204E7A1}"/>
+    <hyperlink ref="D11" r:id="rId9" xr:uid="{B6B41A93-32D6-4188-931A-0BA9EEC1F316}"/>
+    <hyperlink ref="D13" r:id="rId10" xr:uid="{023A60FA-C3A2-4D2A-AE30-8D5DE09DBADF}"/>
+    <hyperlink ref="D14" r:id="rId11" xr:uid="{19F8CEAC-141D-49E5-8EB6-AA7085410473}"/>
+    <hyperlink ref="D15" r:id="rId12" xr:uid="{178243F6-6229-4A27-A26C-4182D5E2F925}"/>
+    <hyperlink ref="D16" r:id="rId13" xr:uid="{C7232B27-B911-4FCF-9105-55F3F5A59091}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2281,64 +2663,64 @@
   <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="B16" sqref="B3:D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="50.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="46.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="94.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" customWidth="1"/>
-    <col min="9" max="9" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="50.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="94.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5546875" customWidth="1"/>
+    <col min="9" max="9" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>78</v>
+        <v>54</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>79</v>
+        <v>55</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>80</v>
+        <v>56</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>81</v>
+        <v>57</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>82</v>
+        <v>58</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>83</v>
+        <v>59</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>84</v>
+        <v>60</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>85</v>
+        <v>61</v>
       </c>
       <c r="J1" s="10" t="s">
-        <v>86</v>
+        <v>62</v>
       </c>
       <c r="K1" s="10" t="s">
-        <v>87</v>
+        <v>63</v>
       </c>
       <c r="L1" s="10" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
@@ -2354,433 +2736,433 @@
       <c r="K2" s="11"/>
       <c r="L2" s="11"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>97</v>
+        <v>151</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>98</v>
+        <v>149</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>163</v>
       </c>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
       <c r="G3" s="11" t="s">
-        <v>126</v>
+        <v>77</v>
       </c>
       <c r="H3" s="11"/>
       <c r="I3" s="11" t="s">
-        <v>95</v>
+        <v>70</v>
       </c>
       <c r="J3" s="11" t="s">
-        <v>92</v>
+        <v>67</v>
       </c>
       <c r="K3" s="11" t="s">
-        <v>127</v>
+        <v>78</v>
       </c>
       <c r="L3" s="11"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>99</v>
+        <v>72</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>100</v>
+        <v>69</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>73</v>
       </c>
       <c r="E4" s="11"/>
       <c r="F4" s="11"/>
       <c r="G4" s="11" t="s">
-        <v>126</v>
+        <v>77</v>
       </c>
       <c r="H4" s="11"/>
       <c r="I4" s="11" t="s">
-        <v>95</v>
+        <v>70</v>
       </c>
       <c r="J4" s="11" t="s">
-        <v>92</v>
+        <v>67</v>
       </c>
       <c r="K4" s="11" t="s">
-        <v>127</v>
+        <v>78</v>
       </c>
       <c r="L4" s="11"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>101</v>
+        <v>74</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>94</v>
+        <v>69</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>102</v>
+        <v>75</v>
       </c>
       <c r="E5" s="11"/>
       <c r="F5" s="11"/>
       <c r="G5" s="11" t="s">
-        <v>126</v>
+        <v>77</v>
       </c>
       <c r="H5" s="11"/>
       <c r="I5" s="11" t="s">
-        <v>95</v>
+        <v>70</v>
       </c>
       <c r="J5" s="11" t="s">
-        <v>92</v>
+        <v>67</v>
       </c>
       <c r="K5" s="11" t="s">
-        <v>127</v>
+        <v>78</v>
       </c>
       <c r="L5" s="11"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>103</v>
+        <v>152</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>104</v>
+        <v>148</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>164</v>
       </c>
       <c r="E6" s="11"/>
       <c r="F6" s="11"/>
       <c r="G6" s="11" t="s">
-        <v>126</v>
+        <v>77</v>
       </c>
       <c r="H6" s="11"/>
       <c r="I6" s="11" t="s">
-        <v>95</v>
+        <v>70</v>
       </c>
       <c r="J6" s="11" t="s">
-        <v>92</v>
+        <v>67</v>
       </c>
       <c r="K6" s="11" t="s">
-        <v>127</v>
+        <v>78</v>
       </c>
       <c r="L6" s="11"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>105</v>
+        <v>153</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>106</v>
+        <v>149</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>165</v>
       </c>
       <c r="E7" s="11"/>
       <c r="F7" s="11"/>
       <c r="G7" s="11" t="s">
-        <v>126</v>
+        <v>77</v>
       </c>
       <c r="H7" s="11"/>
       <c r="I7" s="11" t="s">
-        <v>95</v>
+        <v>70</v>
       </c>
       <c r="J7" s="11" t="s">
-        <v>92</v>
+        <v>67</v>
       </c>
       <c r="K7" s="11" t="s">
-        <v>127</v>
+        <v>78</v>
       </c>
       <c r="L7" s="11"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>107</v>
+        <v>154</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>108</v>
+        <v>149</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>166</v>
       </c>
       <c r="E8" s="11"/>
       <c r="F8" s="11"/>
       <c r="G8" s="11" t="s">
-        <v>128</v>
+        <v>79</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>129</v>
+        <v>80</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>91</v>
+        <v>66</v>
       </c>
       <c r="J8" s="11" t="s">
-        <v>92</v>
+        <v>67</v>
       </c>
       <c r="K8" s="11"/>
       <c r="L8" s="11"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>109</v>
+        <v>155</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>110</v>
+        <v>150</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>147</v>
       </c>
       <c r="E9" s="11"/>
       <c r="F9" s="11"/>
       <c r="G9" s="11" t="s">
-        <v>126</v>
+        <v>77</v>
       </c>
       <c r="H9" s="11"/>
       <c r="I9" s="11" t="s">
-        <v>95</v>
+        <v>70</v>
       </c>
       <c r="J9" s="11" t="s">
-        <v>92</v>
+        <v>67</v>
       </c>
       <c r="K9" s="11" t="s">
-        <v>127</v>
+        <v>78</v>
       </c>
       <c r="L9" s="11"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>111</v>
+        <v>156</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>112</v>
+        <v>149</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>167</v>
       </c>
       <c r="E10" s="11"/>
       <c r="F10" s="11"/>
       <c r="G10" s="11" t="s">
-        <v>126</v>
+        <v>77</v>
       </c>
       <c r="H10" s="11"/>
       <c r="I10" s="11" t="s">
-        <v>95</v>
+        <v>70</v>
       </c>
       <c r="J10" s="11" t="s">
-        <v>92</v>
+        <v>67</v>
       </c>
       <c r="K10" s="11" t="s">
-        <v>127</v>
+        <v>78</v>
       </c>
       <c r="L10" s="11"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>113</v>
+        <v>157</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>114</v>
+        <v>149</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>168</v>
       </c>
       <c r="E11" s="11"/>
       <c r="F11" s="11"/>
       <c r="G11" s="11" t="s">
-        <v>126</v>
+        <v>77</v>
       </c>
       <c r="H11" s="11"/>
       <c r="I11" s="11" t="s">
-        <v>95</v>
+        <v>70</v>
       </c>
       <c r="J11" s="11" t="s">
-        <v>92</v>
+        <v>67</v>
       </c>
       <c r="K11" s="11" t="s">
-        <v>127</v>
+        <v>78</v>
       </c>
       <c r="L11" s="11"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>115</v>
+        <v>158</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>116</v>
+        <v>150</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>146</v>
       </c>
       <c r="E12" s="11"/>
       <c r="F12" s="11"/>
       <c r="G12" s="11" t="s">
-        <v>130</v>
+        <v>81</v>
       </c>
       <c r="H12" s="11" t="s">
-        <v>131</v>
+        <v>82</v>
       </c>
       <c r="I12" s="11" t="s">
-        <v>91</v>
+        <v>66</v>
       </c>
       <c r="J12" s="11" t="s">
-        <v>92</v>
+        <v>67</v>
       </c>
       <c r="K12" s="11" t="s">
-        <v>132</v>
+        <v>83</v>
       </c>
       <c r="L12" s="11"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>117</v>
+        <v>159</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>118</v>
+        <v>149</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>169</v>
       </c>
       <c r="E13" s="11"/>
       <c r="F13" s="11"/>
       <c r="G13" s="11" t="s">
-        <v>133</v>
+        <v>84</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>134</v>
+        <v>85</v>
       </c>
       <c r="I13" s="11" t="s">
-        <v>91</v>
+        <v>66</v>
       </c>
       <c r="J13" s="11" t="s">
-        <v>92</v>
+        <v>67</v>
       </c>
       <c r="K13" s="11" t="s">
-        <v>132</v>
+        <v>83</v>
       </c>
       <c r="L13" s="11"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>119</v>
+        <v>160</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>120</v>
+        <v>149</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>170</v>
       </c>
       <c r="E14" s="11"/>
       <c r="F14" s="11"/>
       <c r="G14" s="11" t="s">
-        <v>126</v>
+        <v>77</v>
       </c>
       <c r="H14" s="11"/>
       <c r="I14" s="11" t="s">
-        <v>95</v>
+        <v>70</v>
       </c>
       <c r="J14" s="11" t="s">
-        <v>92</v>
+        <v>67</v>
       </c>
       <c r="K14" s="11" t="s">
-        <v>127</v>
+        <v>78</v>
       </c>
       <c r="L14" s="11"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>121</v>
+        <v>161</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>122</v>
+        <v>149</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>171</v>
       </c>
       <c r="E15" s="11"/>
       <c r="F15" s="11"/>
       <c r="G15" s="11" t="s">
-        <v>135</v>
+        <v>86</v>
       </c>
       <c r="H15" s="11" t="s">
-        <v>136</v>
+        <v>87</v>
       </c>
       <c r="I15" s="11" t="s">
-        <v>95</v>
+        <v>70</v>
       </c>
       <c r="J15" s="11" t="s">
-        <v>96</v>
+        <v>71</v>
       </c>
       <c r="K15" s="11"/>
       <c r="L15" s="11"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>123</v>
+        <v>162</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>124</v>
+        <v>149</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>172</v>
       </c>
       <c r="E16" s="11"/>
       <c r="F16" s="11"/>
       <c r="G16" s="11" t="s">
-        <v>137</v>
+        <v>88</v>
       </c>
       <c r="H16" s="11" t="s">
-        <v>138</v>
+        <v>89</v>
       </c>
       <c r="I16" s="11" t="s">
-        <v>91</v>
+        <v>66</v>
       </c>
       <c r="J16" s="11" t="s">
-        <v>92</v>
+        <v>67</v>
       </c>
       <c r="K16" s="11"/>
       <c r="L16" s="11"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="B17" s="11"/>
       <c r="C17" s="11"/>
@@ -2795,6 +3177,21 @@
       <c r="L17" s="11"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D9" r:id="rId1" xr:uid="{81137991-E320-42B4-B8F0-196400703443}"/>
+    <hyperlink ref="D12" r:id="rId2" xr:uid="{4961E314-1FF9-481D-BB99-3E2CB1464A7E}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{8D03C335-45A3-4674-9E97-961F662D22C7}"/>
+    <hyperlink ref="D3" r:id="rId4" xr:uid="{7FB8931F-8A11-4A0D-AED5-06DC8AEAC093}"/>
+    <hyperlink ref="D6" r:id="rId5" xr:uid="{CA0AA40D-4241-4D12-90EA-F0EF716670E3}"/>
+    <hyperlink ref="D7" r:id="rId6" xr:uid="{748DEFDD-7654-4216-A702-057A538897F7}"/>
+    <hyperlink ref="D8" r:id="rId7" xr:uid="{479780AD-ECAF-4207-A786-34F06D03665A}"/>
+    <hyperlink ref="D10" r:id="rId8" xr:uid="{07D03400-AF7E-47FE-A53E-56F46C1C6AE7}"/>
+    <hyperlink ref="D11" r:id="rId9" xr:uid="{72A0F295-D37B-464E-954F-C4DDA4818A15}"/>
+    <hyperlink ref="D13" r:id="rId10" xr:uid="{46C936FB-2B07-42DB-A95A-51B02A63E1F8}"/>
+    <hyperlink ref="D14" r:id="rId11" xr:uid="{D6127426-92EE-484F-89BC-63FFE5B18825}"/>
+    <hyperlink ref="D15" r:id="rId12" xr:uid="{7C500A13-BDE3-47FA-B0F0-CF10AD2FDF70}"/>
+    <hyperlink ref="D16" r:id="rId13" xr:uid="{B11C985A-E53F-4B05-8F3E-E1563F43BB28}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>